<commit_message>
Correct run range RGD and add empty target
</commit_message>
<xml_diff>
--- a/rgd_run_range.xlsx
+++ b/rgd_run_range.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathieuouillon/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DD3E113-DA3E-AE4F-A201-2B1BAD0CB211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E13D45-E852-7747-B705-8D39A1A9AA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4380" yWindow="3180" windowWidth="27640" windowHeight="16940" xr2:uid="{69A4BC9E-7DBD-1645-92D6-F9736B030A9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="11">
   <si>
     <t>Target</t>
   </si>
@@ -47,9 +47,6 @@
     <t>End</t>
   </si>
   <si>
-    <t xml:space="preserve">Torus </t>
-  </si>
-  <si>
     <t>LD2</t>
   </si>
   <si>
@@ -63,13 +60,22 @@
   </si>
   <si>
     <t>OB</t>
+  </si>
+  <si>
+    <t>Torus</t>
+  </si>
+  <si>
+    <t>Empty </t>
+  </si>
+  <si>
+    <t>Zero-field </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,17 +85,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,20 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D73730-BCB2-3540-8C4F-4061A1AD25DF}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,273 +466,329 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>18305</v>
       </c>
       <c r="C2" s="1">
-        <v>18336</v>
+        <v>18312</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
-        <v>18339</v>
-      </c>
-      <c r="C3" s="3">
-        <v>18346</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18316</v>
+      </c>
+      <c r="C3" s="1">
+        <v>18316</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>18347</v>
-      </c>
-      <c r="C4" s="3">
-        <v>18368</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>18318</v>
+      </c>
+      <c r="C4" s="1">
+        <v>18336</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>18369</v>
-      </c>
-      <c r="C5" s="3">
-        <v>18371</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>18339</v>
+      </c>
+      <c r="C5" s="1">
+        <v>18346</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>18372</v>
-      </c>
-      <c r="C6" s="2">
-        <v>18394</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>18347</v>
+      </c>
+      <c r="C6" s="1">
+        <v>18368</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>18369</v>
+      </c>
+      <c r="C7" s="1">
+        <v>18371</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" s="2">
-        <v>18400</v>
-      </c>
-      <c r="C7" s="1">
-        <v>18401</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>18372</v>
+      </c>
+      <c r="C8" s="1">
+        <v>18394</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>18419</v>
-      </c>
-      <c r="C8" s="2">
-        <v>18439</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2">
-        <v>18440</v>
-      </c>
-      <c r="C9" s="2">
-        <v>18524</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>18399</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18399</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>18400</v>
+      </c>
+      <c r="C10" s="1">
+        <v>18401</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B10" s="4">
-        <v>18528</v>
-      </c>
-      <c r="C10" s="2">
-        <v>18559</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
-        <v>18560</v>
-      </c>
-      <c r="C11" s="2">
-        <v>18642</v>
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>18419</v>
+      </c>
+      <c r="C11" s="1">
+        <v>18439</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2">
-        <v>18644</v>
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>18440</v>
       </c>
       <c r="C12" s="1">
-        <v>18656</v>
+        <v>18524</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4">
-        <v>18660</v>
-      </c>
-      <c r="C13" s="2">
-        <v>18755</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>18528</v>
+      </c>
+      <c r="C13" s="1">
+        <v>18559</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4">
-        <v>18756</v>
-      </c>
-      <c r="C14" s="2">
-        <v>18762</v>
+      <c r="B14" s="1">
+        <v>18560</v>
+      </c>
+      <c r="C14" s="1">
+        <v>18642</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="2">
-        <v>18764</v>
+        <v>3</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18644</v>
       </c>
       <c r="C15" s="1">
-        <v>18790</v>
+        <v>18656</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="2">
-        <v>18796</v>
-      </c>
-      <c r="C16" s="2">
-        <v>18850</v>
+      <c r="B16" s="1">
+        <v>18660</v>
+      </c>
+      <c r="C16" s="1">
+        <v>18755</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2">
-        <v>18851</v>
-      </c>
-      <c r="C17" s="2">
-        <v>18873</v>
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>18756</v>
+      </c>
+      <c r="C17" s="1">
+        <v>18762</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2">
-        <v>18874</v>
-      </c>
-      <c r="C18" s="2">
-        <v>18966</v>
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>18764</v>
+      </c>
+      <c r="C18" s="1">
+        <v>18790</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="2">
-        <v>19021</v>
-      </c>
-      <c r="C19" s="2">
-        <v>19058</v>
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18796</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18850</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>18851</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18873</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <v>18874</v>
+      </c>
+      <c r="C21" s="1">
+        <v>18966</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>19021</v>
+      </c>
+      <c r="C22" s="1">
+        <v>19058</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>19060</v>
+      </c>
+      <c r="C23" s="1">
+        <v>19060</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1">
         <v>19061</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C24" s="1">
         <v>19131</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rgd ranges and fixed ci
</commit_message>
<xml_diff>
--- a/rgd_run_range.xlsx
+++ b/rgd_run_range.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathieuouillon/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/gemc/clas12Tags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E13D45-E852-7747-B705-8D39A1A9AA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F90C907-AABE-554D-8F34-DB5001C52BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3180" windowWidth="27640" windowHeight="16940" xr2:uid="{69A4BC9E-7DBD-1645-92D6-F9736B030A9F}"/>
+    <workbookView xWindow="65820" yWindow="10620" windowWidth="28320" windowHeight="20660" xr2:uid="{69A4BC9E-7DBD-1645-92D6-F9736B030A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D73730-BCB2-3540-8C4F-4061A1AD25DF}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>